<commit_message>
Uses cases v.3 rendu + html/css index.php
Date du rendu des uses cases.
</commit_message>
<xml_diff>
--- a/Documentation/Journal de bord.xlsx
+++ b/Documentation/Journal de bord.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>Temps</t>
   </si>
@@ -193,6 +193,21 @@
   </si>
   <si>
     <t>Remplir le journal de bord du 01.02.2018 au 13.02.2018</t>
+  </si>
+  <si>
+    <t>Mercredi 14.02.2018</t>
+  </si>
+  <si>
+    <t>Jeudi 15.02.2018</t>
+  </si>
+  <si>
+    <t>Il a été décider de prendre la vidéo trouvée sur youtube au lieu de refaire les uses cases pour les différentes mains et actions possibles</t>
+  </si>
+  <si>
+    <t>Voir avec le chef de projet les uses cases et parler de l'analyse des différents etats dans les quels se trouvent les joueurs</t>
+  </si>
+  <si>
+    <t>Corriger les uses cases avec le chef de projet, regarder avec le chef de projet l'UML qu'il ma fournit afin de voir les différents états d'une main</t>
   </si>
 </sst>
 </file>
@@ -426,90 +441,90 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,1224 +809,1238 @@
   <dimension ref="A1:L162"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" style="20" customWidth="1"/>
-    <col min="3" max="3" width="88.5703125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="73.42578125" style="23" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="88.5703125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="73.42578125" style="12" customWidth="1"/>
     <col min="9" max="10" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="G2" s="1" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="23"/>
+      <c r="G2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="17"/>
+      <c r="G3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6">
+      <c r="H3" s="27"/>
+      <c r="I3" s="2">
         <v>0</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="G4" s="7" t="s">
+      <c r="D4" s="17"/>
+      <c r="G4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="11">
+      <c r="H4" s="29"/>
+      <c r="I4" s="3">
         <v>0.19444444444444445</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="G5" s="7" t="s">
+      <c r="D5" s="17"/>
+      <c r="G5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="11">
+      <c r="H5" s="29"/>
+      <c r="I5" s="3">
         <v>0.10069444444444443</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="G6" s="7" t="s">
+      <c r="D6" s="17"/>
+      <c r="G6" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="11">
+      <c r="H6" s="29"/>
+      <c r="I6" s="3">
         <v>0.13194444444444445</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="G7" s="9" t="s">
+      <c r="D7" s="17"/>
+      <c r="G7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="12">
+      <c r="H7" s="20"/>
+      <c r="I7" s="4">
         <v>0.13194444444444445</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="17" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="23"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="28"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="28"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="28"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="28"/>
+      <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="28"/>
+      <c r="D18" s="17"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="28"/>
+      <c r="D19" s="17"/>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="28"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="28"/>
+      <c r="D21" s="17"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="28"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="28"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="17" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="A25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="17" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="28"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="28"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+      <c r="A29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="28"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="15"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="28"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="28"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="17"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="28"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="28"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="28"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="17"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="17"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="28"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="17"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="21"/>
-      <c r="D37" s="28"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="28"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="17"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="21"/>
-      <c r="D39" s="28"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="17"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="28"/>
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
-      <c r="B41" s="17"/>
-      <c r="C41" s="21"/>
-      <c r="D41" s="28"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="17"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="28"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="17"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="28"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="17"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="28"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="17"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="21"/>
-      <c r="D45" s="28"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="17"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="28"/>
+      <c r="A46" s="5"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="17"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="16"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="28"/>
+      <c r="A47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="17"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="28"/>
+      <c r="A48" s="5"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="17"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="28"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="17"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="21"/>
-      <c r="D50" s="28"/>
+      <c r="A50" s="5"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="17"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="21"/>
-      <c r="D51" s="28"/>
+      <c r="A51" s="5"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="17"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="21"/>
-      <c r="D52" s="28"/>
+      <c r="A52" s="5"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="17"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="28"/>
+      <c r="A53" s="5"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="17"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="21"/>
-      <c r="D54" s="28"/>
+      <c r="A54" s="5"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="17"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="21"/>
-      <c r="D55" s="28"/>
+      <c r="A55" s="5"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="17"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="21"/>
-      <c r="D56" s="28"/>
+      <c r="A56" s="5"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="17"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="21"/>
-      <c r="D57" s="28"/>
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="17"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="21"/>
-      <c r="D58" s="28"/>
+      <c r="A58" s="5"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="17"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="28"/>
+      <c r="A59" s="5"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="17"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="21"/>
-      <c r="D60" s="28"/>
+      <c r="A60" s="5"/>
+      <c r="B60" s="6"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="17"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="16"/>
-      <c r="B61" s="17"/>
-      <c r="C61" s="21"/>
-      <c r="D61" s="28"/>
+      <c r="A61" s="5"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="17"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="16"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="21"/>
-      <c r="D62" s="28"/>
+      <c r="A62" s="5"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="17"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="28"/>
+      <c r="A63" s="5"/>
+      <c r="B63" s="6"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="17"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="21"/>
-      <c r="D64" s="28"/>
+      <c r="A64" s="5"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="16"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="28"/>
+      <c r="A65" s="5"/>
+      <c r="B65" s="6"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="17"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="21"/>
-      <c r="D66" s="28"/>
+      <c r="A66" s="5"/>
+      <c r="B66" s="6"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="21"/>
-      <c r="D67" s="28"/>
+      <c r="A67" s="5"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="17"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
-      <c r="B68" s="17"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="28"/>
+      <c r="A68" s="5"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="17"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="28"/>
+      <c r="A69" s="5"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="17"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="21"/>
-      <c r="D70" s="28"/>
+      <c r="A70" s="5"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="17"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="21"/>
-      <c r="D71" s="28"/>
+      <c r="A71" s="5"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="17"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="28"/>
+      <c r="A72" s="5"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="17"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="21"/>
-      <c r="D73" s="28"/>
+      <c r="A73" s="5"/>
+      <c r="B73" s="6"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="17"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="16"/>
-      <c r="B74" s="17"/>
-      <c r="C74" s="21"/>
-      <c r="D74" s="28"/>
+      <c r="A74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="17"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
-      <c r="B75" s="17"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="28"/>
+      <c r="A75" s="5"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="17"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="21"/>
-      <c r="D76" s="28"/>
+      <c r="A76" s="5"/>
+      <c r="B76" s="6"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="17"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="21"/>
-      <c r="D77" s="28"/>
+      <c r="A77" s="5"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="17"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="16"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="28"/>
+      <c r="A78" s="5"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="17"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="21"/>
-      <c r="D79" s="28"/>
+      <c r="A79" s="5"/>
+      <c r="B79" s="6"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="17"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="21"/>
-      <c r="D80" s="28"/>
+      <c r="A80" s="5"/>
+      <c r="B80" s="6"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="17"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="16"/>
-      <c r="B81" s="17"/>
-      <c r="C81" s="21"/>
-      <c r="D81" s="28"/>
+      <c r="A81" s="5"/>
+      <c r="B81" s="6"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="17"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
-      <c r="B82" s="17"/>
-      <c r="C82" s="21"/>
-      <c r="D82" s="28"/>
+      <c r="A82" s="5"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="17"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
-      <c r="B83" s="17"/>
-      <c r="C83" s="21"/>
-      <c r="D83" s="28"/>
+      <c r="A83" s="5"/>
+      <c r="B83" s="6"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="17"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="16"/>
-      <c r="B84" s="17"/>
-      <c r="C84" s="21"/>
-      <c r="D84" s="28"/>
+      <c r="A84" s="5"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="17"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="16"/>
-      <c r="B85" s="17"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="28"/>
+      <c r="A85" s="5"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="17"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="16"/>
-      <c r="B86" s="17"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="28"/>
+      <c r="A86" s="5"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="17"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="16"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="21"/>
-      <c r="D87" s="28"/>
+      <c r="A87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="17"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="16"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="21"/>
-      <c r="D88" s="28"/>
+      <c r="A88" s="5"/>
+      <c r="B88" s="6"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="17"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="16"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="21"/>
-      <c r="D89" s="28"/>
+      <c r="A89" s="5"/>
+      <c r="B89" s="6"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="17"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
-      <c r="B90" s="17"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="28"/>
+      <c r="A90" s="5"/>
+      <c r="B90" s="6"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="17"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
-      <c r="B91" s="17"/>
-      <c r="C91" s="21"/>
-      <c r="D91" s="28"/>
+      <c r="A91" s="5"/>
+      <c r="B91" s="6"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="17"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
-      <c r="B92" s="17"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="28"/>
+      <c r="A92" s="5"/>
+      <c r="B92" s="6"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="17"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
-      <c r="B93" s="17"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="28"/>
+      <c r="A93" s="5"/>
+      <c r="B93" s="6"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="17"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="16"/>
-      <c r="B94" s="17"/>
-      <c r="C94" s="21"/>
-      <c r="D94" s="28"/>
+      <c r="A94" s="5"/>
+      <c r="B94" s="6"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="17"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="16"/>
-      <c r="B95" s="17"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="28"/>
+      <c r="A95" s="5"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="17"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="16"/>
-      <c r="B96" s="17"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="28"/>
+      <c r="A96" s="5"/>
+      <c r="B96" s="6"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="17"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="16"/>
-      <c r="B97" s="17"/>
-      <c r="C97" s="21"/>
-      <c r="D97" s="28"/>
+      <c r="A97" s="5"/>
+      <c r="B97" s="6"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="17"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="16"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="28"/>
+      <c r="A98" s="5"/>
+      <c r="B98" s="6"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="17"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="16"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="28"/>
+      <c r="A99" s="5"/>
+      <c r="B99" s="6"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="17"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="16"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="28"/>
+      <c r="A100" s="5"/>
+      <c r="B100" s="6"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="17"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="16"/>
-      <c r="B101" s="17"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="28"/>
+      <c r="A101" s="5"/>
+      <c r="B101" s="6"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="17"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="16"/>
-      <c r="B102" s="17"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="28"/>
+      <c r="A102" s="5"/>
+      <c r="B102" s="6"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="17"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="16"/>
-      <c r="B103" s="17"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="28"/>
+      <c r="A103" s="5"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="17"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="16"/>
-      <c r="B104" s="17"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="28"/>
+      <c r="A104" s="5"/>
+      <c r="B104" s="6"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="17"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="16"/>
-      <c r="B105" s="17"/>
-      <c r="C105" s="21"/>
-      <c r="D105" s="28"/>
+      <c r="A105" s="5"/>
+      <c r="B105" s="6"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="17"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="16"/>
-      <c r="B106" s="17"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="28"/>
+      <c r="A106" s="5"/>
+      <c r="B106" s="6"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="17"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="16"/>
-      <c r="B107" s="17"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="28"/>
+      <c r="A107" s="5"/>
+      <c r="B107" s="6"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="17"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="16"/>
-      <c r="B108" s="17"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="28"/>
+      <c r="A108" s="5"/>
+      <c r="B108" s="6"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="17"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="16"/>
-      <c r="B109" s="17"/>
-      <c r="C109" s="21"/>
-      <c r="D109" s="28"/>
+      <c r="A109" s="5"/>
+      <c r="B109" s="6"/>
+      <c r="C109" s="10"/>
+      <c r="D109" s="17"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="16"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="21"/>
-      <c r="D110" s="28"/>
+      <c r="A110" s="5"/>
+      <c r="B110" s="6"/>
+      <c r="C110" s="10"/>
+      <c r="D110" s="17"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="16"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="28"/>
+      <c r="A111" s="5"/>
+      <c r="B111" s="6"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="17"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="16"/>
-      <c r="B112" s="17"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="28"/>
+      <c r="A112" s="5"/>
+      <c r="B112" s="6"/>
+      <c r="C112" s="10"/>
+      <c r="D112" s="17"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="16"/>
-      <c r="B113" s="17"/>
-      <c r="C113" s="21"/>
-      <c r="D113" s="28"/>
+      <c r="A113" s="5"/>
+      <c r="B113" s="6"/>
+      <c r="C113" s="10"/>
+      <c r="D113" s="17"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="16"/>
-      <c r="B114" s="17"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="28"/>
+      <c r="A114" s="5"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="10"/>
+      <c r="D114" s="17"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="16"/>
-      <c r="B115" s="17"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="28"/>
+      <c r="A115" s="5"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="10"/>
+      <c r="D115" s="17"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="16"/>
-      <c r="B116" s="17"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="28"/>
+      <c r="A116" s="5"/>
+      <c r="B116" s="6"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="17"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="16"/>
-      <c r="B117" s="17"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="28"/>
+      <c r="A117" s="5"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="10"/>
+      <c r="D117" s="17"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="16"/>
-      <c r="B118" s="17"/>
-      <c r="C118" s="21"/>
-      <c r="D118" s="28"/>
+      <c r="A118" s="5"/>
+      <c r="B118" s="6"/>
+      <c r="C118" s="10"/>
+      <c r="D118" s="17"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="16"/>
-      <c r="B119" s="17"/>
-      <c r="C119" s="21"/>
-      <c r="D119" s="28"/>
+      <c r="A119" s="5"/>
+      <c r="B119" s="6"/>
+      <c r="C119" s="10"/>
+      <c r="D119" s="17"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="16"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="28"/>
+      <c r="A120" s="5"/>
+      <c r="B120" s="6"/>
+      <c r="C120" s="10"/>
+      <c r="D120" s="17"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="16"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="21"/>
-      <c r="D121" s="28"/>
+      <c r="A121" s="5"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="17"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="16"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="21"/>
-      <c r="D122" s="28"/>
+      <c r="A122" s="5"/>
+      <c r="B122" s="6"/>
+      <c r="C122" s="10"/>
+      <c r="D122" s="17"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="16"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="28"/>
+      <c r="A123" s="5"/>
+      <c r="B123" s="6"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="17"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="16"/>
-      <c r="B124" s="17"/>
-      <c r="C124" s="21"/>
-      <c r="D124" s="28"/>
+      <c r="A124" s="5"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="17"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="16"/>
-      <c r="B125" s="17"/>
-      <c r="C125" s="21"/>
-      <c r="D125" s="28"/>
+      <c r="A125" s="5"/>
+      <c r="B125" s="6"/>
+      <c r="C125" s="10"/>
+      <c r="D125" s="17"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="16"/>
-      <c r="B126" s="17"/>
-      <c r="C126" s="21"/>
-      <c r="D126" s="28"/>
+      <c r="A126" s="5"/>
+      <c r="B126" s="6"/>
+      <c r="C126" s="10"/>
+      <c r="D126" s="17"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="16"/>
-      <c r="B127" s="17"/>
-      <c r="C127" s="21"/>
-      <c r="D127" s="28"/>
+      <c r="A127" s="5"/>
+      <c r="B127" s="6"/>
+      <c r="C127" s="10"/>
+      <c r="D127" s="17"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="16"/>
-      <c r="B128" s="17"/>
-      <c r="C128" s="21"/>
-      <c r="D128" s="28"/>
+      <c r="A128" s="5"/>
+      <c r="B128" s="6"/>
+      <c r="C128" s="10"/>
+      <c r="D128" s="17"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="16"/>
-      <c r="B129" s="17"/>
-      <c r="C129" s="21"/>
-      <c r="D129" s="28"/>
+      <c r="A129" s="5"/>
+      <c r="B129" s="6"/>
+      <c r="C129" s="10"/>
+      <c r="D129" s="17"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="16"/>
-      <c r="B130" s="17"/>
-      <c r="C130" s="21"/>
-      <c r="D130" s="28"/>
+      <c r="A130" s="5"/>
+      <c r="B130" s="6"/>
+      <c r="C130" s="10"/>
+      <c r="D130" s="17"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="16"/>
-      <c r="B131" s="17"/>
-      <c r="C131" s="21"/>
-      <c r="D131" s="28"/>
+      <c r="A131" s="5"/>
+      <c r="B131" s="6"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="17"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="16"/>
-      <c r="B132" s="17"/>
-      <c r="C132" s="21"/>
-      <c r="D132" s="28"/>
+      <c r="A132" s="5"/>
+      <c r="B132" s="6"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="17"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="16"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="21"/>
-      <c r="D133" s="28"/>
+      <c r="A133" s="5"/>
+      <c r="B133" s="6"/>
+      <c r="C133" s="10"/>
+      <c r="D133" s="17"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="16"/>
-      <c r="B134" s="17"/>
-      <c r="C134" s="21"/>
-      <c r="D134" s="28"/>
+      <c r="A134" s="5"/>
+      <c r="B134" s="6"/>
+      <c r="C134" s="10"/>
+      <c r="D134" s="17"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="16"/>
-      <c r="B135" s="17"/>
-      <c r="C135" s="21"/>
-      <c r="D135" s="28"/>
+      <c r="A135" s="5"/>
+      <c r="B135" s="6"/>
+      <c r="C135" s="10"/>
+      <c r="D135" s="17"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="16"/>
-      <c r="B136" s="17"/>
-      <c r="C136" s="21"/>
-      <c r="D136" s="28"/>
+      <c r="A136" s="5"/>
+      <c r="B136" s="6"/>
+      <c r="C136" s="10"/>
+      <c r="D136" s="17"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="16"/>
-      <c r="B137" s="17"/>
-      <c r="C137" s="21"/>
-      <c r="D137" s="28"/>
+      <c r="A137" s="5"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="10"/>
+      <c r="D137" s="17"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="16"/>
-      <c r="B138" s="17"/>
-      <c r="C138" s="21"/>
-      <c r="D138" s="28"/>
+      <c r="A138" s="5"/>
+      <c r="B138" s="6"/>
+      <c r="C138" s="10"/>
+      <c r="D138" s="17"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="16"/>
-      <c r="B139" s="17"/>
-      <c r="C139" s="21"/>
-      <c r="D139" s="28"/>
+      <c r="A139" s="5"/>
+      <c r="B139" s="6"/>
+      <c r="C139" s="10"/>
+      <c r="D139" s="17"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="16"/>
-      <c r="B140" s="17"/>
-      <c r="C140" s="21"/>
-      <c r="D140" s="28"/>
+      <c r="A140" s="5"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="10"/>
+      <c r="D140" s="17"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="16"/>
-      <c r="B141" s="17"/>
-      <c r="C141" s="21"/>
-      <c r="D141" s="28"/>
+      <c r="A141" s="5"/>
+      <c r="B141" s="6"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="17"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="16"/>
-      <c r="B142" s="17"/>
-      <c r="C142" s="21"/>
-      <c r="D142" s="28"/>
+      <c r="A142" s="5"/>
+      <c r="B142" s="6"/>
+      <c r="C142" s="10"/>
+      <c r="D142" s="17"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="16"/>
-      <c r="B143" s="17"/>
-      <c r="C143" s="21"/>
-      <c r="D143" s="28"/>
+      <c r="A143" s="5"/>
+      <c r="B143" s="6"/>
+      <c r="C143" s="10"/>
+      <c r="D143" s="17"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="16"/>
-      <c r="B144" s="17"/>
-      <c r="C144" s="21"/>
-      <c r="D144" s="28"/>
+      <c r="A144" s="5"/>
+      <c r="B144" s="6"/>
+      <c r="C144" s="10"/>
+      <c r="D144" s="17"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="16"/>
-      <c r="B145" s="17"/>
-      <c r="C145" s="21"/>
-      <c r="D145" s="28"/>
+      <c r="A145" s="5"/>
+      <c r="B145" s="6"/>
+      <c r="C145" s="10"/>
+      <c r="D145" s="17"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="16"/>
-      <c r="B146" s="17"/>
-      <c r="C146" s="21"/>
-      <c r="D146" s="28"/>
+      <c r="A146" s="5"/>
+      <c r="B146" s="6"/>
+      <c r="C146" s="10"/>
+      <c r="D146" s="17"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="16"/>
-      <c r="B147" s="17"/>
-      <c r="C147" s="21"/>
-      <c r="D147" s="28"/>
+      <c r="A147" s="5"/>
+      <c r="B147" s="6"/>
+      <c r="C147" s="10"/>
+      <c r="D147" s="17"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="16"/>
-      <c r="B148" s="17"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="28"/>
+      <c r="A148" s="5"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="17"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="16"/>
-      <c r="B149" s="17"/>
-      <c r="C149" s="21"/>
-      <c r="D149" s="28"/>
+      <c r="A149" s="5"/>
+      <c r="B149" s="6"/>
+      <c r="C149" s="10"/>
+      <c r="D149" s="17"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="16"/>
-      <c r="B150" s="17"/>
-      <c r="C150" s="21"/>
-      <c r="D150" s="28"/>
+      <c r="A150" s="5"/>
+      <c r="B150" s="6"/>
+      <c r="C150" s="10"/>
+      <c r="D150" s="17"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="16"/>
-      <c r="B151" s="17"/>
-      <c r="C151" s="21"/>
-      <c r="D151" s="28"/>
+      <c r="A151" s="5"/>
+      <c r="B151" s="6"/>
+      <c r="C151" s="10"/>
+      <c r="D151" s="17"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="16"/>
-      <c r="B152" s="17"/>
-      <c r="C152" s="21"/>
-      <c r="D152" s="28"/>
+      <c r="A152" s="5"/>
+      <c r="B152" s="6"/>
+      <c r="C152" s="10"/>
+      <c r="D152" s="17"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="16"/>
-      <c r="B153" s="17"/>
-      <c r="C153" s="21"/>
-      <c r="D153" s="28"/>
+      <c r="A153" s="5"/>
+      <c r="B153" s="6"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="17"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="16"/>
-      <c r="B154" s="17"/>
-      <c r="C154" s="21"/>
-      <c r="D154" s="28"/>
+      <c r="A154" s="5"/>
+      <c r="B154" s="6"/>
+      <c r="C154" s="10"/>
+      <c r="D154" s="17"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="16"/>
-      <c r="B155" s="17"/>
-      <c r="C155" s="21"/>
-      <c r="D155" s="28"/>
+      <c r="A155" s="5"/>
+      <c r="B155" s="6"/>
+      <c r="C155" s="10"/>
+      <c r="D155" s="17"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="16"/>
-      <c r="B156" s="17"/>
-      <c r="C156" s="21"/>
-      <c r="D156" s="28"/>
+      <c r="A156" s="5"/>
+      <c r="B156" s="6"/>
+      <c r="C156" s="10"/>
+      <c r="D156" s="17"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="16"/>
-      <c r="B157" s="17"/>
-      <c r="C157" s="21"/>
-      <c r="D157" s="28"/>
+      <c r="A157" s="5"/>
+      <c r="B157" s="6"/>
+      <c r="C157" s="10"/>
+      <c r="D157" s="17"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="16"/>
-      <c r="B158" s="17"/>
-      <c r="C158" s="21"/>
-      <c r="D158" s="28"/>
+      <c r="A158" s="5"/>
+      <c r="B158" s="6"/>
+      <c r="C158" s="10"/>
+      <c r="D158" s="17"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="16"/>
-      <c r="B159" s="17"/>
-      <c r="C159" s="21"/>
-      <c r="D159" s="28"/>
+      <c r="A159" s="5"/>
+      <c r="B159" s="6"/>
+      <c r="C159" s="10"/>
+      <c r="D159" s="17"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="16"/>
-      <c r="B160" s="17"/>
-      <c r="C160" s="21"/>
-      <c r="D160" s="28"/>
+      <c r="A160" s="5"/>
+      <c r="B160" s="6"/>
+      <c r="C160" s="10"/>
+      <c r="D160" s="17"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="16"/>
-      <c r="B161" s="17"/>
-      <c r="C161" s="21"/>
-      <c r="D161" s="28"/>
+      <c r="A161" s="5"/>
+      <c r="B161" s="6"/>
+      <c r="C161" s="10"/>
+      <c r="D161" s="17"/>
     </row>
     <row r="162" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="18"/>
-      <c r="B162" s="19"/>
-      <c r="C162" s="22"/>
-      <c r="D162" s="29"/>
+      <c r="A162" s="7"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="11"/>
+      <c r="D162" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>